<commit_message>
Updated Ice Breaber with sample videos; Updated Stakeholder Management sheet - 17/03/2021
</commit_message>
<xml_diff>
--- a/BusinessManagement/StakeholderManagement.xlsx
+++ b/BusinessManagement/StakeholderManagement.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="82">
   <si>
     <t>Anodiam</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Debasish Dutta</t>
   </si>
   <si>
-    <t>20/02/2021: 3:30 PM AUEST</t>
-  </si>
-  <si>
     <t>Icebreaker</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>English</t>
   </si>
   <si>
-    <t>21/02/2021: 6:00 PM AUEST</t>
-  </si>
-  <si>
     <t>Videography</t>
   </si>
   <si>
@@ -145,9 +139,6 @@
     <t>Jayesh Debnath</t>
   </si>
   <si>
-    <t>22/02/2021: 4:30 PM AUEST</t>
-  </si>
-  <si>
     <t>Chemistry</t>
   </si>
   <si>
@@ -208,9 +199,6 @@
     <t xml:space="preserve">26/02/2021: 1.30PM AUST </t>
   </si>
   <si>
-    <t>01/03/2021: 4.00 PM AUST</t>
-  </si>
-  <si>
     <t>Next Steps with Jayesh Debnath</t>
   </si>
   <si>
@@ -226,9 +214,6 @@
     <t>IRC</t>
   </si>
   <si>
-    <t>12/03/2021: 7:30 PM AUEST</t>
-  </si>
-  <si>
     <t>13/03/2021: 2:30 PM AUEST</t>
   </si>
   <si>
@@ -242,6 +227,45 @@
   </si>
   <si>
     <t>05/03/2021: 8:30 PM AUEST</t>
+  </si>
+  <si>
+    <t>Content Creation</t>
+  </si>
+  <si>
+    <t>12/03/2021: 3:30 PM AUEST</t>
+  </si>
+  <si>
+    <t>Recurring Sunday 3:00 PM AUEST</t>
+  </si>
+  <si>
+    <t>21/03/2021: 2:30 PM AUEST</t>
+  </si>
+  <si>
+    <t>Parag Biswas</t>
+  </si>
+  <si>
+    <t>22/03/2021: 7:00 PM AUEST</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Stakeholder Sub Group</t>
+  </si>
+  <si>
+    <t>9 CBSE ICSE</t>
+  </si>
+  <si>
+    <t>9 10 CBSE</t>
+  </si>
+  <si>
+    <t>To start with Planning Spreadsheet</t>
+  </si>
+  <si>
+    <t>Recurring Sunday 8:30 PM AUEST</t>
+  </si>
+  <si>
+    <t>17/03/2021: 7:30 PM AUEST</t>
   </si>
 </sst>
 </file>
@@ -315,12 +339,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -350,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -384,6 +414,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -397,6 +429,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -632,31 +667,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="60" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -726,107 +761,113 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="7" customWidth="1"/>
+    <col min="3" max="3" width="13" style="17" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22" t="s">
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="9" t="s">
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="F3" s="10" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="H3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -834,401 +875,435 @@
         <v>20</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="H4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>51</v>
-      </c>
       <c r="E5" s="10" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>5</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="G7" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>6</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>43</v>
+      <c r="B8" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="10"/>
-    </row>
-    <row r="9" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>7</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>73</v>
+      <c r="E9" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="10"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>8</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="G10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="10" t="s">
+      <c r="I10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>9</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" t="s">
-        <v>61</v>
-      </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="J11" s="13"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K11" s="13"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>10</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>61</v>
-      </c>
       <c r="F12" s="14" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>23</v>
-      </c>
       <c r="G13" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>12</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>67</v>
-      </c>
       <c r="E14" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>13</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="10" t="s">
+      <c r="G15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="I15" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J15" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>14</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="B16" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>60</v>
+      <c r="E16" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="10"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="12"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>15</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>46</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>28</v>
+        <v>43</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="12"/>
-      <c r="I17" s="10"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="12"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>16</v>
       </c>
-      <c r="B18" s="10"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>17</v>
       </c>
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>18</v>
       </c>
       <c r="B20" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>